<commit_message>
Minor improvements to MirrorMe, in preparation of RAMiCS 2017 in Lyon
</commit_message>
<xml_diff>
--- a/MirrorMe/MirrorMe - Stef Example.xlsx
+++ b/MirrorMe/MirrorMe - Stef Example.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
   <si>
     <t>ttScope</t>
   </si>
@@ -74,27 +74,9 @@
     <t>art. 7 WOR</t>
   </si>
   <si>
-    <t>onderneming</t>
-  </si>
-  <si>
-    <t>Belastingdienst</t>
-  </si>
-  <si>
-    <t>bestuurder</t>
-  </si>
-  <si>
-    <t>DG-Bel</t>
-  </si>
-  <si>
     <t>De Belastingdienst is een onderneming in de zin van de Wet op de ondernemingsraden, omdat het een in de maatschappij als zelfstandige eenheid optredend organisatorisch verband is, waarin krachtens arbeidsovereenkomst of krachtens publiekrechtelijke aanstelling arbeid wordt verricht.</t>
   </si>
   <si>
-    <t>Voor de toepassing van het bij of krachtens de WOR bepaalde wordt de [bestuurder] geacht niet te behoren tot de in de [onderneming] werkzame personen.</t>
-  </si>
-  <si>
-    <t>Verkiesbaar tot lid van de ondernemingsraad zijn de personen die gedurende ten minste een jaar in de [onderneming] werkzaam zijn geweest.</t>
-  </si>
-  <si>
     <t>De ondernemingsraad kiest uit zijn midden een voorzitter.</t>
   </si>
   <si>
@@ -104,21 +86,12 @@
     <t>TText_05, TText_06</t>
   </si>
   <si>
-    <t>De DG-Bel is bestuurder in de zin van de Wet op de ondernemingsraden, omdat hij in de [onderneming] de hoogste zeggenschap uitoefent bij de leiding van de arbeid.</t>
-  </si>
-  <si>
     <t>legalGround</t>
   </si>
   <si>
     <t>LegalGround</t>
   </si>
   <si>
-    <t>De [bestuurder] kan geen voorzitter zijn van de ondernemingsraad van de [onderneming].</t>
-  </si>
-  <si>
-    <t>De [bestuurder] is niet verkiesbaar tot lid van de ondernemingsraad van de [onderneming].</t>
-  </si>
-  <si>
     <t>Binding</t>
   </si>
   <si>
@@ -143,33 +116,9 @@
     <t>[Case]</t>
   </si>
   <si>
-    <t>In applying the WOR or any regulation based on the WOR, the [executive officer] is considered not to be part of the workforce of the [enterprise].</t>
-  </si>
-  <si>
-    <t>Eligible as member of the Enterprise Council are persons who have been employed by the [enterprise] for at least a year.</t>
-  </si>
-  <si>
-    <t>The [executive officer] is not eligible as member of the Enterprise Council of the [enterprise].</t>
-  </si>
-  <si>
     <t>The Enterprise Council elects a president from its own members.</t>
   </si>
   <si>
-    <t>The [executive officer] cannot be president of the Enterprise Council of the [enterprise].</t>
-  </si>
-  <si>
-    <t>The Tax Authority is an enterprise as meant by the Law on Enterprise Councils (WOR), because it is an independently operating organisational entity, in which labour is performed on the basis of a labour-contract or based on a public administrative appointment.</t>
-  </si>
-  <si>
-    <t>The DG-Bel is executive officer as meant by the Law on Enterprise Councils (WOR), because he exercises in the [enterprise] the highest authority in managing labour.</t>
-  </si>
-  <si>
-    <t>executive officer</t>
-  </si>
-  <si>
-    <t>enterprise</t>
-  </si>
-  <si>
     <t>Case_X638</t>
   </si>
   <si>
@@ -210,6 +159,63 @@
   </si>
   <si>
     <t>requires</t>
+  </si>
+  <si>
+    <t>Eligible as member of the Enterprise Council are persons who have been employed by [the enterprise] for at least a year.</t>
+  </si>
+  <si>
+    <t>the enterprise</t>
+  </si>
+  <si>
+    <t>the executive officer</t>
+  </si>
+  <si>
+    <t>[the executive officer] cannot be president of the Enterprise Council of [the enterprise].</t>
+  </si>
+  <si>
+    <t>[the executive officer] is not eligible as member of the Enterprise Council of [the enterprise].</t>
+  </si>
+  <si>
+    <t>In applying the WOR or any regulation based on the WOR, [the executive officer] is considered not to be part of the workforce of [the enterprise].</t>
+  </si>
+  <si>
+    <t>de Belastingdienst</t>
+  </si>
+  <si>
+    <t>the Taxation Authority</t>
+  </si>
+  <si>
+    <t>The Taxation Authority is an enterprise as meant by the Law on Enterprise Councils (WOR), because it is an independently operating organisational entity, in which labour is performed on the basis of a labour-contract or based on a public administrative appointment.</t>
+  </si>
+  <si>
+    <t>the Director General of Taxes</t>
+  </si>
+  <si>
+    <t>The Director General of Taxes (DG-Tax) is executive officer as meant by the Law on Enterprise Councils (WOR), because he exercises in [the enterprise] the highest authority in managing labour.</t>
+  </si>
+  <si>
+    <t>de bestuurder</t>
+  </si>
+  <si>
+    <t>de onderneming</t>
+  </si>
+  <si>
+    <t>de DG-Bel</t>
+  </si>
+  <si>
+    <t>De DG-Bel is bestuurder in de zin van de Wet op de ondernemingsraden, omdat hij in [de onderneming] de hoogste zeggenschap uitoefent bij de leiding van de arbeid.</t>
+  </si>
+  <si>
+    <t>Voor de toepassing van het bij of krachtens de WOR bepaalde wordt [de bestuurder] geacht niet te behoren tot de in [de onderneming] werkzame personen.</t>
+  </si>
+  <si>
+    <t>Verkiesbaar tot lid van de ondernemingsraad zijn de personen die gedurende ten minste een jaar in [de onderneming] werkzaam zijn geweest.</t>
+  </si>
+  <si>
+    <t>[de bestuurder] is niet verkiesbaar tot lid van de ondernemingsraad van [de onderneming].</t>
+  </si>
+  <si>
+    <t>[de bestuurder] kan geen voorzitter zijn van de ondernemingsraad van [de onderneming].</t>
   </si>
 </sst>
 </file>
@@ -592,7 +598,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +614,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -623,21 +629,21 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -646,24 +652,24 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C3" s="4">
         <v>3</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>16</v>
@@ -671,17 +677,17 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4">
         <v>4</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>17</v>
@@ -689,33 +695,33 @@
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C5" s="4">
         <v>5</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4">
         <v>6</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>18</v>
@@ -723,24 +729,24 @@
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C7" s="4">
         <v>7</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>0</v>
@@ -755,18 +761,18 @@
         <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>3</v>
@@ -775,44 +781,44 @@
         <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>15</v>
@@ -820,23 +826,23 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B17" s="3">
         <v>638</v>
@@ -854,7 +860,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -869,7 +877,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -884,21 +892,21 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -907,10 +915,10 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -918,13 +926,13 @@
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C3" s="4">
         <v>3</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>16</v>
@@ -935,14 +943,14 @@
         <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4">
         <v>4</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="8" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>17</v>
@@ -953,16 +961,16 @@
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C5" s="4">
         <v>5</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -970,13 +978,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4">
         <v>6</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>18</v>
@@ -987,21 +995,21 @@
         <v>11</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C7" s="4">
         <v>7</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>0</v>
@@ -1016,18 +1024,18 @@
         <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>3</v>
@@ -1036,7 +1044,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1044,16 +1052,16 @@
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>14</v>
@@ -1064,16 +1072,16 @@
         <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>15</v>
@@ -1081,23 +1089,23 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B17" s="3">
         <v>123</v>

</xml_diff>

<commit_message>
Added possibility to qualify a statement as either true or false by claimant party as well as defendant party
</commit_message>
<xml_diff>
--- a/MirrorMe/MirrorMe - Stef Example.xlsx
+++ b/MirrorMe/MirrorMe - Stef Example.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="135" windowWidth="14805" windowHeight="7380" activeTab="1"/>
+    <workbookView xWindow="3408" yWindow="132" windowWidth="14808" windowHeight="7380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MirrorMe Example Argument" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="71">
   <si>
     <t>ttScope</t>
   </si>
@@ -233,7 +233,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -316,6 +316,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -363,7 +366,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -396,9 +399,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -431,6 +451,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -606,25 +643,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="79.42578125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="10.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="79.44140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -647,7 +684,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -670,7 +707,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>35</v>
       </c>
@@ -687,7 +724,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>36</v>
       </c>
@@ -705,7 +742,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
@@ -722,7 +759,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>39</v>
       </c>
@@ -739,7 +776,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>40</v>
       </c>
@@ -756,7 +793,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -776,7 +813,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -796,7 +833,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -816,7 +853,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
@@ -836,7 +873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
@@ -844,7 +881,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
@@ -852,7 +889,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>34</v>
       </c>
@@ -869,25 +906,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="79.42578125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="10.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="79.44140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -910,7 +947,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -933,7 +970,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -950,7 +987,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -968,7 +1005,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -985,7 +1022,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1002,7 +1039,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1019,7 +1056,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -1027,7 +1064,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1047,7 +1084,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1067,7 +1104,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -1087,7 +1124,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1107,7 +1144,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
@@ -1115,7 +1152,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
@@ -1123,7 +1160,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>29</v>
       </c>
@@ -1131,7 +1168,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>68</v>
       </c>
@@ -1139,7 +1176,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>70</v>
       </c>
@@ -1147,7 +1184,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>8</v>
       </c>
@@ -1155,13 +1192,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>24</v>
-      </c>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>